<commit_message>
Beginning estimation now waits for symbolic to complete
</commit_message>
<xml_diff>
--- a/covariate_data2.xlsx
+++ b/covariate_data2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aubertine/Documents/repos/Covariate_Tool/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Documents\repos\Covariate_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BF90FE-8F9E-9A4E-85AE-93E5DF08FE61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2890BA82-6D2C-4066-9A2B-5605A591525E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" activeTab="1" xr2:uid="{D432D790-24C9-2149-9336-E4BB80E6BC53}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{D432D790-24C9-2149-9336-E4BB80E6BC53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -403,13 +403,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E59C35-86CA-6C4E-B67E-5D2D3FB8DD63}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,7 +429,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -449,7 +449,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -469,7 +469,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -489,7 +489,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -509,7 +509,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -529,7 +529,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -549,7 +549,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -569,7 +569,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -589,7 +589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -609,7 +609,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -629,7 +629,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -649,7 +649,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -669,7 +669,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -689,7 +689,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -718,13 +718,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8418401A-F4EB-5B4D-9957-0A4348BEB71E}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E1:E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -738,7 +738,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -752,7 +752,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>11</v>
       </c>
@@ -766,7 +766,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -780,7 +780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -794,7 +794,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -808,7 +808,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -822,7 +822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -836,7 +836,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -850,7 +850,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4</v>
       </c>
@@ -864,7 +864,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0</v>
       </c>
@@ -878,7 +878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4</v>
       </c>
@@ -892,7 +892,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -906,7 +906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -920,7 +920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>

</xml_diff>